<commit_message>
feat(clean_unused_rdv_contexts): add a service that clean unused rdv_contexts after user is removed from an organisation
</commit_message>
<xml_diff>
--- a/docs/resources/Fichier_allocataires_test_-_Drôme.xlsx
+++ b/docs/resources/Fichier_allocataires_test_-_Drôme.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/h0list/code/Holist/rdv-insertion/docs/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/h0list/Documents/import de test rdvi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A10FD8-B62B-9741-8076-55FC34E72F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C2FF5D-72D3-CC43-953A-3FE4471C1091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,9 +21,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
-  <si>
-    <t>N° Allocataire</t>
-  </si>
   <si>
     <t>Civilité</t>
   </si>
@@ -162,6 +159,9 @@
   </si>
   <si>
     <t>id iodas</t>
+  </si>
+  <si>
+    <t>N° CAF</t>
   </si>
 </sst>
 </file>
@@ -630,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -659,123 +659,123 @@
   <sheetData>
     <row r="1" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="30" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="L2" s="13"/>
       <c r="M2" s="13"/>
       <c r="N2" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O2" s="15">
         <v>782605941</v>
@@ -796,27 +796,27 @@
     </row>
     <row r="3" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>38</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
@@ -840,27 +840,27 @@
     </row>
     <row r="4" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>37</v>
-      </c>
       <c r="C4" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>

</xml_diff>

<commit_message>
feat(follow_ups):  Clean unused follow_ups after user is removed from an organisation (#1941)
* feat(follow_ups):  Clean unused follow_ups after user is removed from an organisation 

* fix flaky test

* apply Amines review, merge and rename, fix rename seed
</commit_message>
<xml_diff>
--- a/docs/resources/Fichier_allocataires_test_-_Drôme.xlsx
+++ b/docs/resources/Fichier_allocataires_test_-_Drôme.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/h0list/code/Holist/rdv-insertion/docs/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/h0list/Documents/import de test rdvi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A10FD8-B62B-9741-8076-55FC34E72F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C2FF5D-72D3-CC43-953A-3FE4471C1091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,9 +21,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
-  <si>
-    <t>N° Allocataire</t>
-  </si>
   <si>
     <t>Civilité</t>
   </si>
@@ -162,6 +159,9 @@
   </si>
   <si>
     <t>id iodas</t>
+  </si>
+  <si>
+    <t>N° CAF</t>
   </si>
 </sst>
 </file>
@@ -630,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -659,123 +659,123 @@
   <sheetData>
     <row r="1" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="30" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="L2" s="13"/>
       <c r="M2" s="13"/>
       <c r="N2" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O2" s="15">
         <v>782605941</v>
@@ -796,27 +796,27 @@
     </row>
     <row r="3" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>38</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
@@ -840,27 +840,27 @@
     </row>
     <row r="4" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>37</v>
-      </c>
       <c r="C4" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>

</xml_diff>